<commit_message>
Edit staff card, admin scripts updated
</commit_message>
<xml_diff>
--- a/admin/excel/Staff.xlsx
+++ b/admin/excel/Staff.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>surname</t>
   </si>
@@ -82,6 +82,9 @@
     <t>кандидат хим.наук</t>
   </si>
   <si>
+    <t>baneeva@hppi.troitsk.ru</t>
+  </si>
+  <si>
     <t>Барабанов</t>
   </si>
   <si>
@@ -100,6 +103,9 @@
     <t>Михайлович</t>
   </si>
   <si>
+    <t>belemuk@hppi.troitsk.ru</t>
+  </si>
+  <si>
     <t>Боровиков</t>
   </si>
   <si>
@@ -149,6 +155,9 @@
   </si>
   <si>
     <t>tval@hppi.troitsk.ru</t>
+  </si>
+  <si>
+    <t>Администрация</t>
   </si>
 </sst>
 </file>
@@ -233,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,6 +257,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -270,7 +283,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -344,7 +357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>16</v>
       </c>
@@ -366,16 +379,19 @@
       <c r="G3" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>14683</v>
@@ -387,21 +403,21 @@
         <v>1962</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>27020</v>
@@ -415,22 +431,25 @@
       <c r="G5" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="H5" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>15827</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>1965</v>
@@ -439,18 +458,18 @@
         <v>14</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>22578</v>
@@ -462,21 +481,21 @@
         <v>1984</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>19849</v>
@@ -488,21 +507,21 @@
         <v>1976</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>17697</v>
@@ -517,13 +536,17 @@
         <v>14</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" display="abarab@hppi.troitsk.ru"/>
-    <hyperlink ref="H6" r:id="rId2" display="nbor@hppi.troitsk.ru"/>
+    <hyperlink ref="H3" r:id="rId1" display="baneeva@hppi.troitsk.ru"/>
+    <hyperlink ref="H4" r:id="rId2" display="abarab@hppi.troitsk.ru"/>
+    <hyperlink ref="H6" r:id="rId3" display="nbor@hppi.troitsk.ru"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>